<commit_message>
Improved SLS, to imitate the orignal implementation.
</commit_message>
<xml_diff>
--- a/data_raw/dicts/SLS_dict.xlsx
+++ b/data_raw/dicts/SLS_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096F5C94-5486-429E-90E8-23A8EAC2C8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED53B60-50B0-430C-8469-E7AEC7BB27C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SLS_dict" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>key</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Eine Beispielaufgabe</t>
   </si>
   <si>
-    <t>You will now read several series of words or short phrases. In some of these series, one element has a different rhythm from the others. Therefore, pay special attention to the stresses and accents of the words.&lt;br/&gt; Your task is to judge whether the row contains a rhythmically unsuitable element and, if so, to mark the corresponding element. To do this, simply click on the corresponding word.</t>
-  </si>
-  <si>
     <t>EXAMPLE_FEEDBACK_INCORRECT</t>
   </si>
   <si>
@@ -76,16 +73,6 @@
     <t>FEEDBACK</t>
   </si>
   <si>
-    <t>Salzburg Reading Screening (Berlin Version)</t>
-  </si>
-  <si>
-    <t>Salzburger LeseScreening (Berlin Version)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Im Folgenden werden Ihnen Sätze präsentiert, die einfache Sachverhalte beschreiben. Der Inhalt der Sätze kann wahr oder falsch sein. Bitte entscheiden Sie so korrekt aber auch so schnell wie möglich, ob es sich um eine wahre und damit sinnvolle oder um eine falsche und damit sinnlose Aussage handelt.
-</t>
-  </si>
-  <si>
     <t>Welcome to the Salzburg Reading Screening!</t>
   </si>
   <si>
@@ -114,9 +101,6 @@
   </si>
   <si>
     <t>&lt;span style = "color:green"&gt;Correct!&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>&lt;span style = "color:green"&gt;Richtig!&lt;/span&gt;</t>
   </si>
   <si>
     <t>&lt;span style = "color:red"&gt;The answer was not correct.&lt;/span&gt;</t>
@@ -145,15 +129,35 @@
     <t>Press any key to continue</t>
   </si>
   <si>
-    <t xml:space="preserve">Bei **wahren** Aussagen drücken Sie bitte die “j”-Taste.\\
- Bei **falschen** Aussagen drücken Sie bitte die “f”-Taste .\\Sie können am besten Ihre Zeigefinger für die “f”- und “j”-Tasten benutzen.\\ </t>
-  </si>
-  <si>
-    <t>&lt;span style = "color:red"&gt;Das war leider nicht richtig.&lt;/span&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Es folgen jetzt einige Beispiele zur Übung.\\ Nach jedem Satz bekommen Sie eine Rückmeldung, ob Sie richtig geantwortet haben.
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Im Folgenden werden Ihnen Sätze präsentiert, die **einfache Sachverhalte** beschreiben. Der Inhalt der Sätze kann wahr oder falsch sein. Bitte entscheiden Sie **so korrekt** aber auch **so schnell** wie möglich, ob es sich um eine wahre und damit sinnvolle oder um eine falsche und damit sinnlose Aussage handelt.
+</t>
+  </si>
+  <si>
+    <t>In the following, you will be presented with sentences describing **simple facts**. The content of the sentences can be true or false. Please decide **as correctly** but also **as quickly** as possible whether it is a true and therefore meaningful statement or a false and therefore meaningless one.</t>
+  </si>
+  <si>
+    <t>For **true** statements, please press the **"J"-key** .\\
+ For **false** statements, please press the **"F"-key** .\\You can best use your index fingers for the "F"- and "J"-keys.\\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei **wahren** Aussagen drücken Sie bitte die **“J”-Taste**.\\
+ Bei **falschen** Aussagen drücken Sie bitte die **“F”-Taste** .\\**Bitte legen Sie Ihre Zeigefinger jetzt auf die “F”- und “J”-Taste**.\\ </t>
+  </si>
+  <si>
+    <t>Lesetest</t>
+  </si>
+  <si>
+    <t>Reading Test</t>
+  </si>
+  <si>
+    <t>&lt;span style = "color:green"&gt;richtige Antwort&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span style = "color:red"&gt;falsche Antwort&lt;/span&gt;</t>
   </si>
 </sst>
 </file>
@@ -637,13 +641,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1002,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,46 +1032,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1074,18 +1081,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
@@ -1096,7 +1103,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
@@ -1110,10 +1117,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1140,46 +1147,46 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed some quotes from SLS instructions.
</commit_message>
<xml_diff>
--- a/data_raw/dicts/SLS_dict.xlsx
+++ b/data_raw/dicts/SLS_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B34F4D4-1448-4016-93BD-55927BA05CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F115414-20D5-4186-9195-12B88F456648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SLS_dict" sheetId="1" r:id="rId1"/>
@@ -124,10 +124,6 @@
     <t>In the following, you will be presented with sentences describing **simple facts**. The content of the sentences can be true or false. Please decide **as correctly** but also **as quickly** as possible whether it is a true and therefore meaningful statement or a false and therefore meaningless one.</t>
   </si>
   <si>
-    <t>For **true** statements, please press the **"J"-key** .\\
- For **false** statements, please press the **"F"-key** .\\You can best use your index fingers for the "F"- and "J"-keys.\\</t>
-  </si>
-  <si>
     <t>&lt;span style = "color:green"&gt;richtige Antwort&lt;/span&gt;</t>
   </si>
   <si>
@@ -147,14 +143,18 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Bei **wahren** Aussagen drücken Sie bitte die **“J”-Taste** ("J" für "ja, wahr").\\
- Bei **falschen** Aussagen drücken Sie bitte die **“F”-Taste** ("F" für "falsch") .\\**Bitte legen Sie Ihre Zeigefinger jetzt auf die “F”- und “J”-Taste**.\\ </t>
-  </si>
-  <si>
-    <t>Continue with "F" or "J"</t>
-  </si>
-  <si>
-    <t>Weiter mit „F“ oder „J“</t>
+    <t xml:space="preserve">Bei **wahren** Aussagen drücken Sie bitte die **J-Taste** (für „ja, wahr").\\
+ Bei **falschen** Aussagen drücken Sie bitte die **F-Taste** (für „falsch") .\\**Bitte legen Sie Ihre Zeigefinger jetzt auf die F- und J-Taste**.\\ </t>
+  </si>
+  <si>
+    <t>Weiter mit F oder J</t>
+  </si>
+  <si>
+    <t>Continue with F or J</t>
+  </si>
+  <si>
+    <t>For **true** statements, please press the **J-key** .\\
+ For **false** statements, please press the **F-key** .\\You can best use your index fingers for the F and J keys.\\</t>
   </si>
 </sst>
 </file>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,10 +1047,10 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -1058,7 +1058,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -1069,10 +1069,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1131,10 +1131,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1164,7 +1164,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>25</v>
@@ -1175,7 +1175,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>24</v>
@@ -1197,7 +1197,7 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>41</v>

</xml_diff>